<commit_message>
Edits to the data extracted from Hughes et al.
</commit_message>
<xml_diff>
--- a/HughesReefMatches/Hughes100Reefs.xlsx
+++ b/HughesReefMatches/Hughes100Reefs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1892" uniqueCount="432">
   <si>
     <r>
       <rPr>
@@ -4645,6 +4645,9 @@
   </si>
   <si>
     <t>21.3ºS</t>
+  </si>
+  <si>
+    <t>Size_km2</t>
   </si>
 </sst>
 </file>
@@ -4661,11 +4664,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4941,24 +4946,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
     </xf>
@@ -4967,15 +4954,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -5036,6 +5014,33 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5624,10 +5629,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="38" t="s">
         <v>399</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="38" t="s">
         <v>400</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -5758,16 +5763,16 @@
       </c>
     </row>
     <row r="2" spans="1:47" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="57" t="s">
         <v>397</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -8578,25 +8583,25 @@
       </c>
     </row>
     <row r="36" spans="1:47" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="40"/>
-      <c r="B36" s="46" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41">
+      <c r="C36" s="35"/>
+      <c r="D36" s="35">
         <f>MIN(D3:D35)</f>
         <v>1.4</v>
       </c>
-      <c r="E36" s="41">
+      <c r="E36" s="35">
         <f>MIN(E3:E35)</f>
         <v>-31.5</v>
       </c>
-      <c r="F36" s="42"/>
-      <c r="G36" s="41">
+      <c r="F36" s="36"/>
+      <c r="G36" s="35">
         <f>MIN(G3:G35)</f>
         <v>0</v>
       </c>
-      <c r="H36" s="41">
+      <c r="H36" s="35">
         <f>MIN(H3:H35)</f>
         <v>98.9</v>
       </c>
@@ -8641,25 +8646,25 @@
       <c r="AU36" s="14"/>
     </row>
     <row r="37" spans="1:47" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="40"/>
-      <c r="B37" s="46" t="s">
+      <c r="A37" s="34"/>
+      <c r="B37" s="37" t="s">
         <v>398</v>
       </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41">
+      <c r="C37" s="35"/>
+      <c r="D37" s="35">
         <f>MAX(D3:D35)</f>
         <v>32.5</v>
       </c>
-      <c r="E37" s="41">
+      <c r="E37" s="35">
         <f>MAX(E3:E35)</f>
         <v>-0.5</v>
       </c>
-      <c r="F37" s="42"/>
-      <c r="G37" s="41">
+      <c r="F37" s="36"/>
+      <c r="G37" s="35">
         <f>MAX(G3:G35)</f>
         <v>0</v>
       </c>
-      <c r="H37" s="41">
+      <c r="H37" s="35">
         <f>MAX(H3:H35)</f>
         <v>160.6</v>
       </c>
@@ -8704,14 +8709,14 @@
       <c r="AU37" s="14"/>
     </row>
     <row r="38" spans="1:47" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B38" s="35"/>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
       <c r="I38" s="18"/>
@@ -10656,7 +10661,7 @@
         <f t="shared" si="9"/>
         <v/>
       </c>
-      <c r="F61" s="63" t="s">
+      <c r="F61" s="54" t="s">
         <v>429</v>
       </c>
       <c r="G61" s="9" t="str">
@@ -10896,25 +10901,25 @@
       </c>
     </row>
     <row r="64" spans="1:47" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="40"/>
-      <c r="B64" s="46" t="s">
+      <c r="A64" s="34"/>
+      <c r="B64" s="37" t="s">
         <v>403</v>
       </c>
-      <c r="C64" s="41"/>
-      <c r="D64" s="41">
+      <c r="C64" s="35"/>
+      <c r="D64" s="35">
         <f>MIN(D39:D63)</f>
         <v>1.9</v>
       </c>
-      <c r="E64" s="41">
+      <c r="E64" s="35">
         <f>MIN(E39:E63)</f>
         <v>-28.4</v>
       </c>
-      <c r="F64" s="42"/>
-      <c r="G64" s="41">
+      <c r="F64" s="36"/>
+      <c r="G64" s="35">
         <f>MIN(G39:G63)</f>
         <v>0</v>
       </c>
-      <c r="H64" s="41">
+      <c r="H64" s="35">
         <f>MIN(H39:H63)</f>
         <v>32.4</v>
       </c>
@@ -10959,25 +10964,25 @@
       <c r="AU64" s="3"/>
     </row>
     <row r="65" spans="1:47" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="40"/>
-      <c r="B65" s="46" t="s">
+      <c r="A65" s="34"/>
+      <c r="B65" s="37" t="s">
         <v>404</v>
       </c>
-      <c r="C65" s="41"/>
-      <c r="D65" s="41">
+      <c r="C65" s="35"/>
+      <c r="D65" s="35">
         <f>MAX(D39:D63)</f>
         <v>27.3</v>
       </c>
-      <c r="E65" s="41">
+      <c r="E65" s="35">
         <f>MAX(E39:E63)</f>
         <v>-3.5</v>
       </c>
-      <c r="F65" s="42"/>
-      <c r="G65" s="41">
+      <c r="F65" s="36"/>
+      <c r="G65" s="35">
         <f>MAX(G39:G63)</f>
         <v>0</v>
       </c>
-      <c r="H65" s="41">
+      <c r="H65" s="35">
         <f>MAX(H39:H63)</f>
         <v>123</v>
       </c>
@@ -11022,14 +11027,14 @@
       <c r="AU65" s="3"/>
     </row>
     <row r="66" spans="1:47" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="63" t="s">
         <v>229</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="39"/>
+      <c r="B66" s="64"/>
+      <c r="C66" s="64"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="64"/>
+      <c r="F66" s="65"/>
       <c r="G66" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -11352,7 +11357,7 @@
       <c r="B70" s="14" t="s">
         <v>242</v>
       </c>
-      <c r="C70" s="65" t="s">
+      <c r="C70" s="56" t="s">
         <v>430</v>
       </c>
       <c r="D70" s="9" t="str">
@@ -12749,7 +12754,7 @@
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="F86" s="63" t="s">
+      <c r="F86" s="54" t="s">
         <v>417</v>
       </c>
       <c r="G86" s="9">
@@ -13068,25 +13073,25 @@
       </c>
     </row>
     <row r="90" spans="1:47" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="40"/>
-      <c r="B90" s="46" t="s">
+      <c r="A90" s="34"/>
+      <c r="B90" s="37" t="s">
         <v>405</v>
       </c>
-      <c r="C90" s="41"/>
-      <c r="D90" s="41">
+      <c r="C90" s="35"/>
+      <c r="D90" s="35">
         <f>MIN(D67:D89)</f>
         <v>0.5</v>
       </c>
-      <c r="E90" s="41">
+      <c r="E90" s="35">
         <f>MIN(E67:E89)</f>
         <v>-21.5</v>
       </c>
-      <c r="F90" s="50"/>
-      <c r="G90" s="41">
+      <c r="F90" s="41"/>
+      <c r="G90" s="35">
         <f>MIN(G67:G89)</f>
         <v>-172.4</v>
       </c>
-      <c r="H90" s="41">
+      <c r="H90" s="35">
         <f>MIN(H67:H89)</f>
         <v>134.5</v>
       </c>
@@ -13131,25 +13136,25 @@
       <c r="AU90" s="14"/>
     </row>
     <row r="91" spans="1:47" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="40"/>
-      <c r="B91" s="46" t="s">
+      <c r="A91" s="34"/>
+      <c r="B91" s="37" t="s">
         <v>406</v>
       </c>
-      <c r="C91" s="41"/>
-      <c r="D91" s="41">
+      <c r="C91" s="35"/>
+      <c r="D91" s="35">
         <f>MAX(D67:D89)</f>
         <v>25.5</v>
       </c>
-      <c r="E91" s="41">
+      <c r="E91" s="35">
         <f>MAX(E67:E89)</f>
         <v>-0.5</v>
       </c>
-      <c r="F91" s="50"/>
-      <c r="G91" s="41">
+      <c r="F91" s="41"/>
+      <c r="G91" s="35">
         <f>MAX(G67:G89)</f>
         <v>-77.400000000000006</v>
       </c>
-      <c r="H91" s="41">
+      <c r="H91" s="35">
         <f>MAX(H67:H89)</f>
         <v>178</v>
       </c>
@@ -13194,14 +13199,14 @@
       <c r="AU91" s="14"/>
     </row>
     <row r="92" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="37" t="s">
+      <c r="A92" s="63" t="s">
         <v>312</v>
       </c>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="39"/>
+      <c r="B92" s="64"/>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
+      <c r="F92" s="65"/>
       <c r="G92" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -15454,61 +15459,61 @@
       </c>
     </row>
     <row r="116" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B116" s="46" t="s">
+      <c r="B116" s="37" t="s">
         <v>407</v>
       </c>
-      <c r="D116" s="41">
+      <c r="D116" s="35">
         <f>MIN(D93:D115)</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="E116" s="41">
+      <c r="E116" s="35">
         <f>MIN(E93:E115)</f>
         <v>0</v>
       </c>
-      <c r="G116" s="41">
+      <c r="G116" s="35">
         <f>MIN(G93:G115)</f>
         <v>-93.8</v>
       </c>
-      <c r="H116" s="41">
+      <c r="H116" s="35">
         <f>MIN(H93:H115)</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B117" s="46" t="s">
+      <c r="B117" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="D117" s="41">
+      <c r="D117" s="35">
         <f>MAX(D93:D115)</f>
         <v>32.200000000000003</v>
       </c>
-      <c r="E117" s="41">
+      <c r="E117" s="35">
         <f>MAX(E93:E115)</f>
         <v>0</v>
       </c>
-      <c r="G117" s="41">
+      <c r="G117" s="35">
         <f>MAX(G93:G115)</f>
         <v>-59.5</v>
       </c>
-      <c r="H117" s="41">
+      <c r="H117" s="35">
         <f>MAX(H93:H115)</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="G118" s="49"/>
-      <c r="H118" s="49"/>
+      <c r="G118" s="40"/>
+      <c r="H118" s="40"/>
     </row>
     <row r="119" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="G119" s="49"/>
-      <c r="H119" s="49"/>
+      <c r="G119" s="40"/>
+      <c r="H119" s="40"/>
     </row>
     <row r="120" spans="1:47" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B120" s="58" t="s">
+      <c r="B120" s="49" t="s">
         <v>409</v>
       </c>
-      <c r="G120" s="49"/>
-      <c r="H120" s="49"/>
+      <c r="G120" s="40"/>
+      <c r="H120" s="40"/>
     </row>
     <row r="121" spans="1:47" x14ac:dyDescent="0.2">
       <c r="D121" t="s">
@@ -15517,13 +15522,13 @@
       <c r="E121" t="s">
         <v>411</v>
       </c>
-      <c r="F121" s="61" t="s">
+      <c r="F121" s="52" t="s">
         <v>414</v>
       </c>
-      <c r="G121" s="49" t="s">
+      <c r="G121" s="40" t="s">
         <v>412</v>
       </c>
-      <c r="H121" s="49" t="s">
+      <c r="H121" s="40" t="s">
         <v>413</v>
       </c>
       <c r="I121" t="s">
@@ -15531,23 +15536,23 @@
       </c>
     </row>
     <row r="122" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B122" s="56" t="s">
+      <c r="B122" s="47" t="s">
         <v>396</v>
       </c>
-      <c r="C122" s="51"/>
-      <c r="D122" s="51">
+      <c r="C122" s="42"/>
+      <c r="D122" s="42">
         <v>1.4</v>
       </c>
-      <c r="E122" s="51">
+      <c r="E122" s="42">
         <v>-31.5</v>
       </c>
-      <c r="F122" s="51">
+      <c r="F122" s="42">
         <v>-31.5</v>
       </c>
-      <c r="G122" s="52">
+      <c r="G122" s="43">
         <v>0</v>
       </c>
-      <c r="H122" s="52">
+      <c r="H122" s="43">
         <v>98.9</v>
       </c>
       <c r="I122">
@@ -15555,7 +15560,7 @@
       </c>
     </row>
     <row r="123" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B123" s="57" t="s">
+      <c r="B123" s="48" t="s">
         <v>398</v>
       </c>
       <c r="D123">
@@ -15567,10 +15572,10 @@
       <c r="F123">
         <v>32.5</v>
       </c>
-      <c r="G123" s="49">
+      <c r="G123" s="40">
         <v>0</v>
       </c>
-      <c r="H123" s="49">
+      <c r="H123" s="40">
         <v>160.6</v>
       </c>
       <c r="I123">
@@ -15578,7 +15583,7 @@
       </c>
     </row>
     <row r="124" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B124" s="57" t="s">
+      <c r="B124" s="48" t="s">
         <v>403</v>
       </c>
       <c r="D124">
@@ -15590,10 +15595,10 @@
       <c r="F124">
         <v>-28.4</v>
       </c>
-      <c r="G124" s="49">
+      <c r="G124" s="40">
         <v>0</v>
       </c>
-      <c r="H124" s="49">
+      <c r="H124" s="40">
         <v>32.4</v>
       </c>
       <c r="I124">
@@ -15601,7 +15606,7 @@
       </c>
     </row>
     <row r="125" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B125" s="57" t="s">
+      <c r="B125" s="48" t="s">
         <v>404</v>
       </c>
       <c r="D125">
@@ -15613,10 +15618,10 @@
       <c r="F125">
         <v>27.3</v>
       </c>
-      <c r="G125" s="49">
+      <c r="G125" s="40">
         <v>0</v>
       </c>
-      <c r="H125" s="49">
+      <c r="H125" s="40">
         <v>123</v>
       </c>
       <c r="I125">
@@ -15624,7 +15629,7 @@
       </c>
     </row>
     <row r="126" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B126" s="57" t="s">
+      <c r="B126" s="48" t="s">
         <v>405</v>
       </c>
       <c r="D126">
@@ -15636,10 +15641,10 @@
       <c r="F126">
         <v>-21.5</v>
       </c>
-      <c r="G126" s="49">
+      <c r="G126" s="40">
         <v>-172.4</v>
       </c>
-      <c r="H126" s="49">
+      <c r="H126" s="40">
         <v>134.5</v>
       </c>
       <c r="I126" t="s">
@@ -15647,7 +15652,7 @@
       </c>
     </row>
     <row r="127" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B127" s="57" t="s">
+      <c r="B127" s="48" t="s">
         <v>406</v>
       </c>
       <c r="D127">
@@ -15659,33 +15664,33 @@
       <c r="F127">
         <v>25.5</v>
       </c>
-      <c r="G127" s="49">
+      <c r="G127" s="40">
         <v>-77.400000000000006</v>
       </c>
-      <c r="H127" s="49">
+      <c r="H127" s="40">
         <v>178</v>
       </c>
-      <c r="I127" s="61" t="s">
+      <c r="I127" s="52" t="s">
         <v>418</v>
       </c>
     </row>
     <row r="128" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="B128" s="59" t="s">
+      <c r="B128" s="50" t="s">
         <v>407</v>
       </c>
-      <c r="D128" s="53">
+      <c r="D128" s="44">
         <v>9.3000000000000007</v>
       </c>
-      <c r="E128" s="53">
+      <c r="E128" s="44">
         <v>0</v>
       </c>
       <c r="F128">
         <v>9.3000000000000007</v>
       </c>
-      <c r="G128" s="53">
+      <c r="G128" s="44">
         <v>-93.8</v>
       </c>
-      <c r="H128" s="53">
+      <c r="H128" s="44">
         <v>0</v>
       </c>
       <c r="I128">
@@ -15693,23 +15698,23 @@
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B129" s="60" t="s">
+      <c r="B129" s="51" t="s">
         <v>408</v>
       </c>
-      <c r="C129" s="54"/>
-      <c r="D129" s="55">
+      <c r="C129" s="45"/>
+      <c r="D129" s="46">
         <v>32.200000000000003</v>
       </c>
-      <c r="E129" s="55">
+      <c r="E129" s="46">
         <v>0</v>
       </c>
-      <c r="F129" s="54">
+      <c r="F129" s="45">
         <v>32.200000000000003</v>
       </c>
-      <c r="G129" s="55">
+      <c r="G129" s="46">
         <v>-59.5</v>
       </c>
-      <c r="H129" s="55">
+      <c r="H129" s="46">
         <v>0</v>
       </c>
       <c r="I129">
@@ -15717,868 +15722,868 @@
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G130" s="49"/>
-      <c r="H130" s="49"/>
+      <c r="G130" s="40"/>
+      <c r="H130" s="40"/>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G131" s="49"/>
-      <c r="H131" s="49"/>
+      <c r="G131" s="40"/>
+      <c r="H131" s="40"/>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G132" s="49">
+      <c r="G132" s="40">
         <v>-172.4</v>
       </c>
-      <c r="H132" s="49">
+      <c r="H132" s="40">
         <v>134.5</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G133" s="49">
+      <c r="G133" s="40">
         <v>-77.400000000000006</v>
       </c>
-      <c r="H133" s="49">
+      <c r="H133" s="40">
         <v>178</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G134" s="49"/>
-      <c r="H134" s="49"/>
+      <c r="G134" s="40"/>
+      <c r="H134" s="40"/>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G135" s="49"/>
-      <c r="H135" s="49"/>
+      <c r="G135" s="40"/>
+      <c r="H135" s="40"/>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G136" s="49"/>
-      <c r="H136" s="49"/>
+      <c r="G136" s="40"/>
+      <c r="H136" s="40"/>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G137" s="49"/>
-      <c r="H137" s="49"/>
+      <c r="G137" s="40"/>
+      <c r="H137" s="40"/>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G138" s="49"/>
-      <c r="H138" s="49"/>
+      <c r="G138" s="40"/>
+      <c r="H138" s="40"/>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G139" s="49"/>
-      <c r="H139" s="49"/>
+      <c r="G139" s="40"/>
+      <c r="H139" s="40"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G140" s="49"/>
-      <c r="H140" s="49"/>
+      <c r="G140" s="40"/>
+      <c r="H140" s="40"/>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G141" s="49"/>
-      <c r="H141" s="49"/>
+      <c r="G141" s="40"/>
+      <c r="H141" s="40"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G142" s="49"/>
-      <c r="H142" s="49"/>
+      <c r="G142" s="40"/>
+      <c r="H142" s="40"/>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G143" s="49"/>
-      <c r="H143" s="49"/>
+      <c r="G143" s="40"/>
+      <c r="H143" s="40"/>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="G144" s="49"/>
-      <c r="H144" s="49"/>
+      <c r="G144" s="40"/>
+      <c r="H144" s="40"/>
     </row>
     <row r="145" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G145" s="49"/>
-      <c r="H145" s="49"/>
+      <c r="G145" s="40"/>
+      <c r="H145" s="40"/>
     </row>
     <row r="146" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G146" s="49"/>
-      <c r="H146" s="49"/>
+      <c r="G146" s="40"/>
+      <c r="H146" s="40"/>
     </row>
     <row r="147" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G147" s="49"/>
-      <c r="H147" s="49"/>
+      <c r="G147" s="40"/>
+      <c r="H147" s="40"/>
     </row>
     <row r="148" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G148" s="49"/>
-      <c r="H148" s="49"/>
+      <c r="G148" s="40"/>
+      <c r="H148" s="40"/>
     </row>
     <row r="149" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G149" s="49"/>
-      <c r="H149" s="49"/>
+      <c r="G149" s="40"/>
+      <c r="H149" s="40"/>
     </row>
     <row r="150" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G150" s="49"/>
-      <c r="H150" s="49"/>
+      <c r="G150" s="40"/>
+      <c r="H150" s="40"/>
     </row>
     <row r="151" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G151" s="49"/>
-      <c r="H151" s="49"/>
+      <c r="G151" s="40"/>
+      <c r="H151" s="40"/>
     </row>
     <row r="152" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G152" s="49"/>
-      <c r="H152" s="49"/>
+      <c r="G152" s="40"/>
+      <c r="H152" s="40"/>
     </row>
     <row r="153" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G153" s="49"/>
-      <c r="H153" s="49"/>
+      <c r="G153" s="40"/>
+      <c r="H153" s="40"/>
     </row>
     <row r="154" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G154" s="49"/>
-      <c r="H154" s="49"/>
+      <c r="G154" s="40"/>
+      <c r="H154" s="40"/>
     </row>
     <row r="155" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G155" s="49"/>
-      <c r="H155" s="49"/>
+      <c r="G155" s="40"/>
+      <c r="H155" s="40"/>
     </row>
     <row r="156" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G156" s="49"/>
-      <c r="H156" s="49"/>
+      <c r="G156" s="40"/>
+      <c r="H156" s="40"/>
     </row>
     <row r="157" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G157" s="49"/>
-      <c r="H157" s="49"/>
+      <c r="G157" s="40"/>
+      <c r="H157" s="40"/>
     </row>
     <row r="158" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G158" s="49"/>
-      <c r="H158" s="49"/>
+      <c r="G158" s="40"/>
+      <c r="H158" s="40"/>
     </row>
     <row r="159" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G159" s="49"/>
-      <c r="H159" s="49"/>
+      <c r="G159" s="40"/>
+      <c r="H159" s="40"/>
     </row>
     <row r="160" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G160" s="49"/>
-      <c r="H160" s="49"/>
+      <c r="G160" s="40"/>
+      <c r="H160" s="40"/>
     </row>
     <row r="161" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G161" s="49"/>
-      <c r="H161" s="49"/>
+      <c r="G161" s="40"/>
+      <c r="H161" s="40"/>
     </row>
     <row r="162" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G162" s="49"/>
-      <c r="H162" s="49"/>
+      <c r="G162" s="40"/>
+      <c r="H162" s="40"/>
     </row>
     <row r="163" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G163" s="49"/>
-      <c r="H163" s="49"/>
+      <c r="G163" s="40"/>
+      <c r="H163" s="40"/>
     </row>
     <row r="164" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G164" s="49"/>
-      <c r="H164" s="49"/>
+      <c r="G164" s="40"/>
+      <c r="H164" s="40"/>
     </row>
     <row r="165" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G165" s="49"/>
-      <c r="H165" s="49"/>
+      <c r="G165" s="40"/>
+      <c r="H165" s="40"/>
     </row>
     <row r="166" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G166" s="49"/>
-      <c r="H166" s="49"/>
+      <c r="G166" s="40"/>
+      <c r="H166" s="40"/>
     </row>
     <row r="167" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G167" s="49"/>
-      <c r="H167" s="49"/>
+      <c r="G167" s="40"/>
+      <c r="H167" s="40"/>
     </row>
     <row r="168" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G168" s="49"/>
-      <c r="H168" s="49"/>
+      <c r="G168" s="40"/>
+      <c r="H168" s="40"/>
     </row>
     <row r="169" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G169" s="49"/>
-      <c r="H169" s="49"/>
+      <c r="G169" s="40"/>
+      <c r="H169" s="40"/>
     </row>
     <row r="170" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G170" s="49"/>
-      <c r="H170" s="49"/>
+      <c r="G170" s="40"/>
+      <c r="H170" s="40"/>
     </row>
     <row r="171" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G171" s="49"/>
-      <c r="H171" s="49"/>
+      <c r="G171" s="40"/>
+      <c r="H171" s="40"/>
     </row>
     <row r="172" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G172" s="49"/>
-      <c r="H172" s="49"/>
+      <c r="G172" s="40"/>
+      <c r="H172" s="40"/>
     </row>
     <row r="173" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G173" s="49"/>
-      <c r="H173" s="49"/>
+      <c r="G173" s="40"/>
+      <c r="H173" s="40"/>
     </row>
     <row r="174" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G174" s="49"/>
-      <c r="H174" s="49"/>
+      <c r="G174" s="40"/>
+      <c r="H174" s="40"/>
     </row>
     <row r="175" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G175" s="49"/>
-      <c r="H175" s="49"/>
+      <c r="G175" s="40"/>
+      <c r="H175" s="40"/>
     </row>
     <row r="176" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G176" s="49"/>
-      <c r="H176" s="49"/>
+      <c r="G176" s="40"/>
+      <c r="H176" s="40"/>
     </row>
     <row r="177" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G177" s="49"/>
-      <c r="H177" s="49"/>
+      <c r="G177" s="40"/>
+      <c r="H177" s="40"/>
     </row>
     <row r="178" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G178" s="49"/>
-      <c r="H178" s="49"/>
+      <c r="G178" s="40"/>
+      <c r="H178" s="40"/>
     </row>
     <row r="179" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G179" s="49"/>
-      <c r="H179" s="49"/>
+      <c r="G179" s="40"/>
+      <c r="H179" s="40"/>
     </row>
     <row r="180" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G180" s="49"/>
-      <c r="H180" s="49"/>
+      <c r="G180" s="40"/>
+      <c r="H180" s="40"/>
     </row>
     <row r="181" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G181" s="49"/>
-      <c r="H181" s="49"/>
+      <c r="G181" s="40"/>
+      <c r="H181" s="40"/>
     </row>
     <row r="182" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G182" s="49"/>
-      <c r="H182" s="49"/>
+      <c r="G182" s="40"/>
+      <c r="H182" s="40"/>
     </row>
     <row r="183" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G183" s="49"/>
-      <c r="H183" s="49"/>
+      <c r="G183" s="40"/>
+      <c r="H183" s="40"/>
     </row>
     <row r="184" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G184" s="49"/>
-      <c r="H184" s="49"/>
+      <c r="G184" s="40"/>
+      <c r="H184" s="40"/>
     </row>
     <row r="185" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G185" s="49"/>
-      <c r="H185" s="49"/>
+      <c r="G185" s="40"/>
+      <c r="H185" s="40"/>
     </row>
     <row r="186" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G186" s="49"/>
-      <c r="H186" s="49"/>
+      <c r="G186" s="40"/>
+      <c r="H186" s="40"/>
     </row>
     <row r="187" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G187" s="49"/>
-      <c r="H187" s="49"/>
+      <c r="G187" s="40"/>
+      <c r="H187" s="40"/>
     </row>
     <row r="188" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G188" s="49"/>
-      <c r="H188" s="49"/>
+      <c r="G188" s="40"/>
+      <c r="H188" s="40"/>
     </row>
     <row r="189" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G189" s="49"/>
-      <c r="H189" s="49"/>
+      <c r="G189" s="40"/>
+      <c r="H189" s="40"/>
     </row>
     <row r="190" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G190" s="49"/>
-      <c r="H190" s="49"/>
+      <c r="G190" s="40"/>
+      <c r="H190" s="40"/>
     </row>
     <row r="191" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G191" s="49"/>
-      <c r="H191" s="49"/>
+      <c r="G191" s="40"/>
+      <c r="H191" s="40"/>
     </row>
     <row r="192" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G192" s="49"/>
-      <c r="H192" s="49"/>
+      <c r="G192" s="40"/>
+      <c r="H192" s="40"/>
     </row>
     <row r="193" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G193" s="49"/>
-      <c r="H193" s="49"/>
+      <c r="G193" s="40"/>
+      <c r="H193" s="40"/>
     </row>
     <row r="194" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G194" s="49"/>
-      <c r="H194" s="49"/>
+      <c r="G194" s="40"/>
+      <c r="H194" s="40"/>
     </row>
     <row r="195" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G195" s="49"/>
-      <c r="H195" s="49"/>
+      <c r="G195" s="40"/>
+      <c r="H195" s="40"/>
     </row>
     <row r="196" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G196" s="49"/>
-      <c r="H196" s="49"/>
+      <c r="G196" s="40"/>
+      <c r="H196" s="40"/>
     </row>
     <row r="197" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G197" s="49"/>
-      <c r="H197" s="49"/>
+      <c r="G197" s="40"/>
+      <c r="H197" s="40"/>
     </row>
     <row r="198" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G198" s="49"/>
-      <c r="H198" s="49"/>
+      <c r="G198" s="40"/>
+      <c r="H198" s="40"/>
     </row>
     <row r="199" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G199" s="49"/>
-      <c r="H199" s="49"/>
+      <c r="G199" s="40"/>
+      <c r="H199" s="40"/>
     </row>
     <row r="200" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G200" s="49"/>
-      <c r="H200" s="49"/>
+      <c r="G200" s="40"/>
+      <c r="H200" s="40"/>
     </row>
     <row r="201" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G201" s="49"/>
-      <c r="H201" s="49"/>
+      <c r="G201" s="40"/>
+      <c r="H201" s="40"/>
     </row>
     <row r="202" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G202" s="49"/>
-      <c r="H202" s="49"/>
+      <c r="G202" s="40"/>
+      <c r="H202" s="40"/>
     </row>
     <row r="203" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G203" s="49"/>
-      <c r="H203" s="49"/>
+      <c r="G203" s="40"/>
+      <c r="H203" s="40"/>
     </row>
     <row r="204" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G204" s="49"/>
-      <c r="H204" s="49"/>
+      <c r="G204" s="40"/>
+      <c r="H204" s="40"/>
     </row>
     <row r="205" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G205" s="49"/>
-      <c r="H205" s="49"/>
+      <c r="G205" s="40"/>
+      <c r="H205" s="40"/>
     </row>
     <row r="206" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G206" s="49"/>
-      <c r="H206" s="49"/>
+      <c r="G206" s="40"/>
+      <c r="H206" s="40"/>
     </row>
     <row r="207" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G207" s="49"/>
-      <c r="H207" s="49"/>
+      <c r="G207" s="40"/>
+      <c r="H207" s="40"/>
     </row>
     <row r="208" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G208" s="49"/>
-      <c r="H208" s="49"/>
+      <c r="G208" s="40"/>
+      <c r="H208" s="40"/>
     </row>
     <row r="209" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G209" s="49"/>
-      <c r="H209" s="49"/>
+      <c r="G209" s="40"/>
+      <c r="H209" s="40"/>
     </row>
     <row r="210" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G210" s="49"/>
-      <c r="H210" s="49"/>
+      <c r="G210" s="40"/>
+      <c r="H210" s="40"/>
     </row>
     <row r="211" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G211" s="49"/>
-      <c r="H211" s="49"/>
+      <c r="G211" s="40"/>
+      <c r="H211" s="40"/>
     </row>
     <row r="212" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G212" s="49"/>
-      <c r="H212" s="49"/>
+      <c r="G212" s="40"/>
+      <c r="H212" s="40"/>
     </row>
     <row r="213" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G213" s="49"/>
-      <c r="H213" s="49"/>
+      <c r="G213" s="40"/>
+      <c r="H213" s="40"/>
     </row>
     <row r="214" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G214" s="49"/>
-      <c r="H214" s="49"/>
+      <c r="G214" s="40"/>
+      <c r="H214" s="40"/>
     </row>
     <row r="215" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G215" s="49"/>
-      <c r="H215" s="49"/>
+      <c r="G215" s="40"/>
+      <c r="H215" s="40"/>
     </row>
     <row r="216" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G216" s="49"/>
-      <c r="H216" s="49"/>
+      <c r="G216" s="40"/>
+      <c r="H216" s="40"/>
     </row>
     <row r="217" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G217" s="49"/>
-      <c r="H217" s="49"/>
+      <c r="G217" s="40"/>
+      <c r="H217" s="40"/>
     </row>
     <row r="218" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G218" s="49"/>
-      <c r="H218" s="49"/>
+      <c r="G218" s="40"/>
+      <c r="H218" s="40"/>
     </row>
     <row r="219" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G219" s="49"/>
-      <c r="H219" s="49"/>
+      <c r="G219" s="40"/>
+      <c r="H219" s="40"/>
     </row>
     <row r="220" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G220" s="49"/>
-      <c r="H220" s="49"/>
+      <c r="G220" s="40"/>
+      <c r="H220" s="40"/>
     </row>
     <row r="221" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G221" s="49"/>
-      <c r="H221" s="49"/>
+      <c r="G221" s="40"/>
+      <c r="H221" s="40"/>
     </row>
     <row r="222" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G222" s="49"/>
-      <c r="H222" s="49"/>
+      <c r="G222" s="40"/>
+      <c r="H222" s="40"/>
     </row>
     <row r="223" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G223" s="49"/>
-      <c r="H223" s="49"/>
+      <c r="G223" s="40"/>
+      <c r="H223" s="40"/>
     </row>
     <row r="224" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G224" s="49"/>
-      <c r="H224" s="49"/>
+      <c r="G224" s="40"/>
+      <c r="H224" s="40"/>
     </row>
     <row r="225" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G225" s="49"/>
-      <c r="H225" s="49"/>
+      <c r="G225" s="40"/>
+      <c r="H225" s="40"/>
     </row>
     <row r="226" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G226" s="49"/>
-      <c r="H226" s="49"/>
+      <c r="G226" s="40"/>
+      <c r="H226" s="40"/>
     </row>
     <row r="227" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G227" s="49"/>
-      <c r="H227" s="49"/>
+      <c r="G227" s="40"/>
+      <c r="H227" s="40"/>
     </row>
     <row r="228" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G228" s="49"/>
-      <c r="H228" s="49"/>
+      <c r="G228" s="40"/>
+      <c r="H228" s="40"/>
     </row>
     <row r="229" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G229" s="49"/>
-      <c r="H229" s="49"/>
+      <c r="G229" s="40"/>
+      <c r="H229" s="40"/>
     </row>
     <row r="230" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G230" s="49"/>
-      <c r="H230" s="49"/>
+      <c r="G230" s="40"/>
+      <c r="H230" s="40"/>
     </row>
     <row r="231" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G231" s="49"/>
-      <c r="H231" s="49"/>
+      <c r="G231" s="40"/>
+      <c r="H231" s="40"/>
     </row>
     <row r="232" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G232" s="49"/>
-      <c r="H232" s="49"/>
+      <c r="G232" s="40"/>
+      <c r="H232" s="40"/>
     </row>
     <row r="233" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G233" s="49"/>
-      <c r="H233" s="49"/>
+      <c r="G233" s="40"/>
+      <c r="H233" s="40"/>
     </row>
     <row r="234" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G234" s="49"/>
-      <c r="H234" s="49"/>
+      <c r="G234" s="40"/>
+      <c r="H234" s="40"/>
     </row>
     <row r="235" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G235" s="49"/>
-      <c r="H235" s="49"/>
+      <c r="G235" s="40"/>
+      <c r="H235" s="40"/>
     </row>
     <row r="236" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G236" s="49"/>
-      <c r="H236" s="49"/>
+      <c r="G236" s="40"/>
+      <c r="H236" s="40"/>
     </row>
     <row r="237" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G237" s="49"/>
-      <c r="H237" s="49"/>
+      <c r="G237" s="40"/>
+      <c r="H237" s="40"/>
     </row>
     <row r="238" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G238" s="49"/>
-      <c r="H238" s="49"/>
+      <c r="G238" s="40"/>
+      <c r="H238" s="40"/>
     </row>
     <row r="239" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G239" s="49"/>
-      <c r="H239" s="49"/>
+      <c r="G239" s="40"/>
+      <c r="H239" s="40"/>
     </row>
     <row r="240" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G240" s="49"/>
-      <c r="H240" s="49"/>
+      <c r="G240" s="40"/>
+      <c r="H240" s="40"/>
     </row>
     <row r="241" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G241" s="49"/>
-      <c r="H241" s="49"/>
+      <c r="G241" s="40"/>
+      <c r="H241" s="40"/>
     </row>
     <row r="242" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G242" s="49"/>
-      <c r="H242" s="49"/>
+      <c r="G242" s="40"/>
+      <c r="H242" s="40"/>
     </row>
     <row r="243" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G243" s="49"/>
-      <c r="H243" s="49"/>
+      <c r="G243" s="40"/>
+      <c r="H243" s="40"/>
     </row>
     <row r="244" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G244" s="49"/>
-      <c r="H244" s="49"/>
+      <c r="G244" s="40"/>
+      <c r="H244" s="40"/>
     </row>
     <row r="245" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G245" s="49"/>
-      <c r="H245" s="49"/>
+      <c r="G245" s="40"/>
+      <c r="H245" s="40"/>
     </row>
     <row r="246" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G246" s="49"/>
-      <c r="H246" s="49"/>
+      <c r="G246" s="40"/>
+      <c r="H246" s="40"/>
     </row>
     <row r="247" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G247" s="49"/>
-      <c r="H247" s="49"/>
+      <c r="G247" s="40"/>
+      <c r="H247" s="40"/>
     </row>
     <row r="248" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G248" s="49"/>
-      <c r="H248" s="49"/>
+      <c r="G248" s="40"/>
+      <c r="H248" s="40"/>
     </row>
     <row r="249" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G249" s="49"/>
-      <c r="H249" s="49"/>
+      <c r="G249" s="40"/>
+      <c r="H249" s="40"/>
     </row>
     <row r="250" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G250" s="49"/>
-      <c r="H250" s="49"/>
+      <c r="G250" s="40"/>
+      <c r="H250" s="40"/>
     </row>
     <row r="251" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G251" s="49"/>
-      <c r="H251" s="49"/>
+      <c r="G251" s="40"/>
+      <c r="H251" s="40"/>
     </row>
     <row r="252" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G252" s="49"/>
-      <c r="H252" s="49"/>
+      <c r="G252" s="40"/>
+      <c r="H252" s="40"/>
     </row>
     <row r="253" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G253" s="49"/>
-      <c r="H253" s="49"/>
+      <c r="G253" s="40"/>
+      <c r="H253" s="40"/>
     </row>
     <row r="254" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G254" s="49"/>
-      <c r="H254" s="49"/>
+      <c r="G254" s="40"/>
+      <c r="H254" s="40"/>
     </row>
     <row r="255" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G255" s="49"/>
-      <c r="H255" s="49"/>
+      <c r="G255" s="40"/>
+      <c r="H255" s="40"/>
     </row>
     <row r="256" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G256" s="49"/>
-      <c r="H256" s="49"/>
+      <c r="G256" s="40"/>
+      <c r="H256" s="40"/>
     </row>
     <row r="257" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G257" s="49"/>
-      <c r="H257" s="49"/>
+      <c r="G257" s="40"/>
+      <c r="H257" s="40"/>
     </row>
     <row r="258" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G258" s="49"/>
-      <c r="H258" s="49"/>
+      <c r="G258" s="40"/>
+      <c r="H258" s="40"/>
     </row>
     <row r="259" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G259" s="49"/>
-      <c r="H259" s="49"/>
+      <c r="G259" s="40"/>
+      <c r="H259" s="40"/>
     </row>
     <row r="260" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G260" s="49"/>
-      <c r="H260" s="49"/>
+      <c r="G260" s="40"/>
+      <c r="H260" s="40"/>
     </row>
     <row r="261" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G261" s="49"/>
-      <c r="H261" s="49"/>
+      <c r="G261" s="40"/>
+      <c r="H261" s="40"/>
     </row>
     <row r="262" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G262" s="49"/>
-      <c r="H262" s="49"/>
+      <c r="G262" s="40"/>
+      <c r="H262" s="40"/>
     </row>
     <row r="263" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G263" s="49"/>
-      <c r="H263" s="49"/>
+      <c r="G263" s="40"/>
+      <c r="H263" s="40"/>
     </row>
     <row r="264" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G264" s="49"/>
-      <c r="H264" s="49"/>
+      <c r="G264" s="40"/>
+      <c r="H264" s="40"/>
     </row>
     <row r="265" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G265" s="49"/>
-      <c r="H265" s="49"/>
+      <c r="G265" s="40"/>
+      <c r="H265" s="40"/>
     </row>
     <row r="266" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G266" s="49"/>
-      <c r="H266" s="49"/>
+      <c r="G266" s="40"/>
+      <c r="H266" s="40"/>
     </row>
     <row r="267" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G267" s="49"/>
-      <c r="H267" s="49"/>
+      <c r="G267" s="40"/>
+      <c r="H267" s="40"/>
     </row>
     <row r="268" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G268" s="49"/>
-      <c r="H268" s="49"/>
+      <c r="G268" s="40"/>
+      <c r="H268" s="40"/>
     </row>
     <row r="269" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G269" s="49"/>
-      <c r="H269" s="49"/>
+      <c r="G269" s="40"/>
+      <c r="H269" s="40"/>
     </row>
     <row r="270" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G270" s="49"/>
-      <c r="H270" s="49"/>
+      <c r="G270" s="40"/>
+      <c r="H270" s="40"/>
     </row>
     <row r="271" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G271" s="49"/>
-      <c r="H271" s="49"/>
+      <c r="G271" s="40"/>
+      <c r="H271" s="40"/>
     </row>
     <row r="272" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G272" s="49"/>
-      <c r="H272" s="49"/>
+      <c r="G272" s="40"/>
+      <c r="H272" s="40"/>
     </row>
     <row r="273" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G273" s="49"/>
-      <c r="H273" s="49"/>
+      <c r="G273" s="40"/>
+      <c r="H273" s="40"/>
     </row>
     <row r="274" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G274" s="49"/>
-      <c r="H274" s="49"/>
+      <c r="G274" s="40"/>
+      <c r="H274" s="40"/>
     </row>
     <row r="275" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G275" s="49"/>
-      <c r="H275" s="49"/>
+      <c r="G275" s="40"/>
+      <c r="H275" s="40"/>
     </row>
     <row r="276" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G276" s="49"/>
-      <c r="H276" s="49"/>
+      <c r="G276" s="40"/>
+      <c r="H276" s="40"/>
     </row>
     <row r="277" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G277" s="49"/>
-      <c r="H277" s="49"/>
+      <c r="G277" s="40"/>
+      <c r="H277" s="40"/>
     </row>
     <row r="278" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G278" s="49"/>
-      <c r="H278" s="49"/>
+      <c r="G278" s="40"/>
+      <c r="H278" s="40"/>
     </row>
     <row r="279" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G279" s="49"/>
-      <c r="H279" s="49"/>
+      <c r="G279" s="40"/>
+      <c r="H279" s="40"/>
     </row>
     <row r="280" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G280" s="49"/>
-      <c r="H280" s="49"/>
+      <c r="G280" s="40"/>
+      <c r="H280" s="40"/>
     </row>
     <row r="281" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G281" s="49"/>
-      <c r="H281" s="49"/>
+      <c r="G281" s="40"/>
+      <c r="H281" s="40"/>
     </row>
     <row r="282" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G282" s="49"/>
-      <c r="H282" s="49"/>
+      <c r="G282" s="40"/>
+      <c r="H282" s="40"/>
     </row>
     <row r="283" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G283" s="49"/>
-      <c r="H283" s="49"/>
+      <c r="G283" s="40"/>
+      <c r="H283" s="40"/>
     </row>
     <row r="284" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G284" s="49"/>
-      <c r="H284" s="49"/>
+      <c r="G284" s="40"/>
+      <c r="H284" s="40"/>
     </row>
     <row r="285" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G285" s="49"/>
-      <c r="H285" s="49"/>
+      <c r="G285" s="40"/>
+      <c r="H285" s="40"/>
     </row>
     <row r="286" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G286" s="49"/>
-      <c r="H286" s="49"/>
+      <c r="G286" s="40"/>
+      <c r="H286" s="40"/>
     </row>
     <row r="287" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G287" s="49"/>
-      <c r="H287" s="49"/>
+      <c r="G287" s="40"/>
+      <c r="H287" s="40"/>
     </row>
     <row r="288" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G288" s="49"/>
-      <c r="H288" s="49"/>
+      <c r="G288" s="40"/>
+      <c r="H288" s="40"/>
     </row>
     <row r="289" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G289" s="49"/>
-      <c r="H289" s="49"/>
+      <c r="G289" s="40"/>
+      <c r="H289" s="40"/>
     </row>
     <row r="290" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G290" s="49"/>
-      <c r="H290" s="49"/>
+      <c r="G290" s="40"/>
+      <c r="H290" s="40"/>
     </row>
     <row r="291" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G291" s="49"/>
-      <c r="H291" s="49"/>
+      <c r="G291" s="40"/>
+      <c r="H291" s="40"/>
     </row>
     <row r="292" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G292" s="49"/>
-      <c r="H292" s="49"/>
+      <c r="G292" s="40"/>
+      <c r="H292" s="40"/>
     </row>
     <row r="293" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G293" s="49"/>
-      <c r="H293" s="49"/>
+      <c r="G293" s="40"/>
+      <c r="H293" s="40"/>
     </row>
     <row r="294" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G294" s="49"/>
-      <c r="H294" s="49"/>
+      <c r="G294" s="40"/>
+      <c r="H294" s="40"/>
     </row>
     <row r="295" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G295" s="49"/>
-      <c r="H295" s="49"/>
+      <c r="G295" s="40"/>
+      <c r="H295" s="40"/>
     </row>
     <row r="296" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G296" s="49"/>
-      <c r="H296" s="49"/>
+      <c r="G296" s="40"/>
+      <c r="H296" s="40"/>
     </row>
     <row r="297" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G297" s="49"/>
-      <c r="H297" s="49"/>
+      <c r="G297" s="40"/>
+      <c r="H297" s="40"/>
     </row>
     <row r="298" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G298" s="49"/>
-      <c r="H298" s="49"/>
+      <c r="G298" s="40"/>
+      <c r="H298" s="40"/>
     </row>
     <row r="299" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G299" s="49"/>
-      <c r="H299" s="49"/>
+      <c r="G299" s="40"/>
+      <c r="H299" s="40"/>
     </row>
     <row r="300" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G300" s="49"/>
-      <c r="H300" s="49"/>
+      <c r="G300" s="40"/>
+      <c r="H300" s="40"/>
     </row>
     <row r="301" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G301" s="49"/>
-      <c r="H301" s="49"/>
+      <c r="G301" s="40"/>
+      <c r="H301" s="40"/>
     </row>
     <row r="302" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G302" s="49"/>
-      <c r="H302" s="49"/>
+      <c r="G302" s="40"/>
+      <c r="H302" s="40"/>
     </row>
     <row r="303" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G303" s="49"/>
-      <c r="H303" s="49"/>
+      <c r="G303" s="40"/>
+      <c r="H303" s="40"/>
     </row>
     <row r="304" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G304" s="49"/>
-      <c r="H304" s="49"/>
+      <c r="G304" s="40"/>
+      <c r="H304" s="40"/>
     </row>
     <row r="305" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G305" s="49"/>
-      <c r="H305" s="49"/>
+      <c r="G305" s="40"/>
+      <c r="H305" s="40"/>
     </row>
     <row r="306" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G306" s="49"/>
-      <c r="H306" s="49"/>
+      <c r="G306" s="40"/>
+      <c r="H306" s="40"/>
     </row>
     <row r="307" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G307" s="49"/>
-      <c r="H307" s="49"/>
+      <c r="G307" s="40"/>
+      <c r="H307" s="40"/>
     </row>
     <row r="308" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G308" s="49"/>
-      <c r="H308" s="49"/>
+      <c r="G308" s="40"/>
+      <c r="H308" s="40"/>
     </row>
     <row r="309" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G309" s="49"/>
-      <c r="H309" s="49"/>
+      <c r="G309" s="40"/>
+      <c r="H309" s="40"/>
     </row>
     <row r="310" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G310" s="49"/>
-      <c r="H310" s="49"/>
+      <c r="G310" s="40"/>
+      <c r="H310" s="40"/>
     </row>
     <row r="311" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G311" s="49"/>
-      <c r="H311" s="49"/>
+      <c r="G311" s="40"/>
+      <c r="H311" s="40"/>
     </row>
     <row r="312" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G312" s="49"/>
-      <c r="H312" s="49"/>
+      <c r="G312" s="40"/>
+      <c r="H312" s="40"/>
     </row>
     <row r="313" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G313" s="49"/>
-      <c r="H313" s="49"/>
+      <c r="G313" s="40"/>
+      <c r="H313" s="40"/>
     </row>
     <row r="314" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G314" s="49"/>
-      <c r="H314" s="49"/>
+      <c r="G314" s="40"/>
+      <c r="H314" s="40"/>
     </row>
     <row r="315" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G315" s="49"/>
-      <c r="H315" s="49"/>
+      <c r="G315" s="40"/>
+      <c r="H315" s="40"/>
     </row>
     <row r="316" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G316" s="49"/>
-      <c r="H316" s="49"/>
+      <c r="G316" s="40"/>
+      <c r="H316" s="40"/>
     </row>
     <row r="317" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G317" s="49"/>
-      <c r="H317" s="49"/>
+      <c r="G317" s="40"/>
+      <c r="H317" s="40"/>
     </row>
     <row r="318" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G318" s="49"/>
-      <c r="H318" s="49"/>
+      <c r="G318" s="40"/>
+      <c r="H318" s="40"/>
     </row>
     <row r="319" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G319" s="49"/>
-      <c r="H319" s="49"/>
+      <c r="G319" s="40"/>
+      <c r="H319" s="40"/>
     </row>
     <row r="320" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G320" s="49"/>
-      <c r="H320" s="49"/>
+      <c r="G320" s="40"/>
+      <c r="H320" s="40"/>
     </row>
     <row r="321" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G321" s="49"/>
-      <c r="H321" s="49"/>
+      <c r="G321" s="40"/>
+      <c r="H321" s="40"/>
     </row>
     <row r="322" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G322" s="49"/>
-      <c r="H322" s="49"/>
+      <c r="G322" s="40"/>
+      <c r="H322" s="40"/>
     </row>
     <row r="323" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G323" s="49"/>
-      <c r="H323" s="49"/>
+      <c r="G323" s="40"/>
+      <c r="H323" s="40"/>
     </row>
     <row r="324" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G324" s="49"/>
-      <c r="H324" s="49"/>
+      <c r="G324" s="40"/>
+      <c r="H324" s="40"/>
     </row>
     <row r="325" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G325" s="49"/>
-      <c r="H325" s="49"/>
+      <c r="G325" s="40"/>
+      <c r="H325" s="40"/>
     </row>
     <row r="326" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G326" s="49"/>
-      <c r="H326" s="49"/>
+      <c r="G326" s="40"/>
+      <c r="H326" s="40"/>
     </row>
     <row r="327" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G327" s="49"/>
-      <c r="H327" s="49"/>
+      <c r="G327" s="40"/>
+      <c r="H327" s="40"/>
     </row>
     <row r="328" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G328" s="49"/>
-      <c r="H328" s="49"/>
+      <c r="G328" s="40"/>
+      <c r="H328" s="40"/>
     </row>
     <row r="329" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G329" s="49"/>
-      <c r="H329" s="49"/>
+      <c r="G329" s="40"/>
+      <c r="H329" s="40"/>
     </row>
     <row r="330" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G330" s="49"/>
-      <c r="H330" s="49"/>
+      <c r="G330" s="40"/>
+      <c r="H330" s="40"/>
     </row>
     <row r="331" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G331" s="49"/>
-      <c r="H331" s="49"/>
+      <c r="G331" s="40"/>
+      <c r="H331" s="40"/>
     </row>
     <row r="332" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G332" s="49"/>
-      <c r="H332" s="49"/>
+      <c r="G332" s="40"/>
+      <c r="H332" s="40"/>
     </row>
     <row r="333" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G333" s="49"/>
-      <c r="H333" s="49"/>
+      <c r="G333" s="40"/>
+      <c r="H333" s="40"/>
     </row>
     <row r="334" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G334" s="49"/>
-      <c r="H334" s="49"/>
+      <c r="G334" s="40"/>
+      <c r="H334" s="40"/>
     </row>
     <row r="335" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G335" s="49"/>
-      <c r="H335" s="49"/>
+      <c r="G335" s="40"/>
+      <c r="H335" s="40"/>
     </row>
     <row r="336" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G336" s="49"/>
-      <c r="H336" s="49"/>
+      <c r="G336" s="40"/>
+      <c r="H336" s="40"/>
     </row>
     <row r="337" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G337" s="49"/>
-      <c r="H337" s="49"/>
+      <c r="G337" s="40"/>
+      <c r="H337" s="40"/>
     </row>
     <row r="338" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G338" s="49"/>
-      <c r="H338" s="49"/>
+      <c r="G338" s="40"/>
+      <c r="H338" s="40"/>
     </row>
     <row r="339" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G339" s="49"/>
-      <c r="H339" s="49"/>
+      <c r="G339" s="40"/>
+      <c r="H339" s="40"/>
     </row>
     <row r="340" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G340" s="49"/>
-      <c r="H340" s="49"/>
+      <c r="G340" s="40"/>
+      <c r="H340" s="40"/>
     </row>
     <row r="341" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G341" s="49"/>
-      <c r="H341" s="49"/>
+      <c r="G341" s="40"/>
+      <c r="H341" s="40"/>
     </row>
     <row r="342" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G342" s="49"/>
-      <c r="H342" s="49"/>
+      <c r="G342" s="40"/>
+      <c r="H342" s="40"/>
     </row>
     <row r="343" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G343" s="49"/>
-      <c r="H343" s="49"/>
+      <c r="G343" s="40"/>
+      <c r="H343" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -16597,8 +16602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16607,23 +16612,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="53" t="s">
         <v>428</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="53" t="s">
         <v>423</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="38" t="s">
         <v>419</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="38" t="s">
         <v>422</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
+      <c r="F1" s="5" t="s">
+        <v>431</v>
       </c>
       <c r="G1" s="4">
         <v>1980</v>
@@ -16736,10 +16741,10 @@
       <c r="AQ1" s="4">
         <v>2016</v>
       </c>
-      <c r="AR1" s="64" t="s">
+      <c r="AR1" s="55" t="s">
         <v>420</v>
       </c>
-      <c r="AS1" s="64" t="s">
+      <c r="AS1" s="55" t="s">
         <v>421</v>
       </c>
     </row>
@@ -16808,11 +16813,11 @@
         <v>9</v>
       </c>
       <c r="AR2">
-        <f>COUNTIF(G2:AQ2,"S")</f>
+        <f t="shared" ref="AR2:AR33" si="0">COUNTIF(G2:AQ2,"S")</f>
         <v>3</v>
       </c>
       <c r="AS2">
-        <f>COUNTIF(G2:AQ2,"M")</f>
+        <f t="shared" ref="AS2:AS33" si="1">COUNTIF(G2:AQ2,"M")</f>
         <v>1</v>
       </c>
     </row>
@@ -16875,11 +16880,11 @@
         <v>10</v>
       </c>
       <c r="AR3">
-        <f>COUNTIF(G3:AQ3,"S")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AS3">
-        <f>COUNTIF(G3:AQ3,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -16956,11 +16961,11 @@
         <v>9</v>
       </c>
       <c r="AR4">
-        <f>COUNTIF(G4:AQ4,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS4">
-        <f>COUNTIF(G4:AQ4,"M")</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -17031,11 +17036,11 @@
         <v>9</v>
       </c>
       <c r="AR5">
-        <f>COUNTIF(G5:AQ5,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS5">
-        <f>COUNTIF(G5:AQ5,"M")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -17104,11 +17109,11 @@
         <v>10</v>
       </c>
       <c r="AR6">
-        <f>COUNTIF(G6:AQ6,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS6">
-        <f>COUNTIF(G6:AQ6,"M")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -17171,11 +17176,11 @@
         <v>9</v>
       </c>
       <c r="AR7">
-        <f>COUNTIF(G7:AQ7,"S")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AS7">
-        <f>COUNTIF(G7:AQ7,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -17246,11 +17251,11 @@
       <c r="AP8" s="18"/>
       <c r="AQ8" s="18"/>
       <c r="AR8">
-        <f>COUNTIF(G8:AQ8,"S")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AS8">
-        <f>COUNTIF(G8:AQ8,"M")</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
@@ -17321,11 +17326,11 @@
         <v>10</v>
       </c>
       <c r="AR9">
-        <f>COUNTIF(G9:AQ9,"S")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AS9">
-        <f>COUNTIF(G9:AQ9,"M")</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -17390,11 +17395,11 @@
         <v>10</v>
       </c>
       <c r="AR10">
-        <f>COUNTIF(G10:AQ10,"S")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AS10">
-        <f>COUNTIF(G10:AQ10,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -17461,11 +17466,11 @@
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3"/>
       <c r="AR11">
-        <f>COUNTIF(G11:AQ11,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS11">
-        <f>COUNTIF(G11:AQ11,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -17542,11 +17547,11 @@
         <v>9</v>
       </c>
       <c r="AR12">
-        <f>COUNTIF(G12:AQ12,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS12">
-        <f>COUNTIF(G12:AQ12,"M")</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -17611,11 +17616,11 @@
         <v>9</v>
       </c>
       <c r="AR13">
-        <f>COUNTIF(G13:AQ13,"S")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AS13">
-        <f>COUNTIF(G13:AQ13,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -17678,11 +17683,11 @@
       <c r="AP14" s="3"/>
       <c r="AQ14" s="3"/>
       <c r="AR14">
-        <f>COUNTIF(G14:AQ14,"S")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AS14">
-        <f>COUNTIF(G14:AQ14,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -17747,11 +17752,11 @@
         <v>9</v>
       </c>
       <c r="AR15">
-        <f>COUNTIF(G15:AQ15,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS15">
-        <f>COUNTIF(G15:AQ15,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -17816,11 +17821,11 @@
         <v>9</v>
       </c>
       <c r="AR16">
-        <f>COUNTIF(G16:AQ16,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS16">
-        <f>COUNTIF(G16:AQ16,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -17891,11 +17896,11 @@
         <v>9</v>
       </c>
       <c r="AR17">
-        <f>COUNTIF(G17:AQ17,"S")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AS17">
-        <f>COUNTIF(G17:AQ17,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -17962,11 +17967,11 @@
         <v>10</v>
       </c>
       <c r="AR18">
-        <f>COUNTIF(G18:AQ18,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS18">
-        <f>COUNTIF(G18:AQ18,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -18035,11 +18040,11 @@
         <v>9</v>
       </c>
       <c r="AR19">
-        <f>COUNTIF(G19:AQ19,"S")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AS19">
-        <f>COUNTIF(G19:AQ19,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -18106,11 +18111,11 @@
         <v>9</v>
       </c>
       <c r="AR20">
-        <f>COUNTIF(G20:AQ20,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS20">
-        <f>COUNTIF(G20:AQ20,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -18179,11 +18184,11 @@
         <v>9</v>
       </c>
       <c r="AR21">
-        <f>COUNTIF(G21:AQ21,"S")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AS21">
-        <f>COUNTIF(G21:AQ21,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -18248,11 +18253,11 @@
         <v>9</v>
       </c>
       <c r="AR22">
-        <f>COUNTIF(G22:AQ22,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS22">
-        <f>COUNTIF(G22:AQ22,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -18319,11 +18324,11 @@
         <v>9</v>
       </c>
       <c r="AR23">
-        <f>COUNTIF(G23:AQ23,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS23">
-        <f>COUNTIF(G23:AQ23,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -18390,11 +18395,11 @@
         <v>9</v>
       </c>
       <c r="AR24">
-        <f>COUNTIF(G24:AQ24,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS24">
-        <f>COUNTIF(G24:AQ24,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -18461,11 +18466,11 @@
       <c r="AP25" s="18"/>
       <c r="AQ25" s="18"/>
       <c r="AR25">
-        <f>COUNTIF(G25:AQ25,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS25">
-        <f>COUNTIF(G25:AQ25,"M")</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -18556,11 +18561,11 @@
         <v>9</v>
       </c>
       <c r="AR26">
-        <f>COUNTIF(G26:AQ26,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS26">
-        <f>COUNTIF(G26:AQ26,"M")</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
@@ -18627,11 +18632,11 @@
         <v>9</v>
       </c>
       <c r="AR27">
-        <f>COUNTIF(G27:AQ27,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS27">
-        <f>COUNTIF(G27:AQ27,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -18706,11 +18711,11 @@
       <c r="AP28" s="18"/>
       <c r="AQ28" s="18"/>
       <c r="AR28">
-        <f>COUNTIF(G28:AQ28,"S")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AS28">
-        <f>COUNTIF(G28:AQ28,"M")</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
@@ -18795,11 +18800,11 @@
         <v>9</v>
       </c>
       <c r="AR29">
-        <f>COUNTIF(G29:AQ29,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS29">
-        <f>COUNTIF(G29:AQ29,"M")</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
@@ -18870,11 +18875,11 @@
         <v>10</v>
       </c>
       <c r="AR30">
-        <f>COUNTIF(G30:AQ30,"S")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AS30">
-        <f>COUNTIF(G30:AQ30,"M")</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -18953,11 +18958,11 @@
         <v>9</v>
       </c>
       <c r="AR31">
-        <f>COUNTIF(G31:AQ31,"S")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AS31">
-        <f>COUNTIF(G31:AQ31,"M")</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
@@ -19030,11 +19035,11 @@
         <v>9</v>
       </c>
       <c r="AR32">
-        <f>COUNTIF(G32:AQ32,"S")</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="AS32">
-        <f>COUNTIF(G32:AQ32,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -19103,11 +19108,11 @@
         <v>9</v>
       </c>
       <c r="AR33">
-        <f>COUNTIF(G33:AQ33,"S")</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="AS33">
-        <f>COUNTIF(G33:AQ33,"M")</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -19176,11 +19181,11 @@
         <v>10</v>
       </c>
       <c r="AR34">
-        <f>COUNTIF(G34:AQ34,"S")</f>
+        <f t="shared" ref="AR34:AR65" si="2">COUNTIF(G34:AQ34,"S")</f>
         <v>0</v>
       </c>
       <c r="AS34">
-        <f>COUNTIF(G34:AQ34,"M")</f>
+        <f t="shared" ref="AS34:AS65" si="3">COUNTIF(G34:AQ34,"M")</f>
         <v>4</v>
       </c>
     </row>
@@ -19251,11 +19256,11 @@
         <v>9</v>
       </c>
       <c r="AR35">
-        <f>COUNTIF(G35:AQ35,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS35">
-        <f>COUNTIF(G35:AQ35,"M")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -19324,11 +19329,11 @@
         <v>10</v>
       </c>
       <c r="AR36">
-        <f>COUNTIF(G36:AQ36,"S")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS36">
-        <f>COUNTIF(G36:AQ36,"M")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -19393,11 +19398,11 @@
         <v>10</v>
       </c>
       <c r="AR37">
-        <f>COUNTIF(G37:AQ37,"S")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS37">
-        <f>COUNTIF(G37:AQ37,"M")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -19466,11 +19471,11 @@
         <v>9</v>
       </c>
       <c r="AR38">
-        <f>COUNTIF(G38:AQ38,"S")</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AS38">
-        <f>COUNTIF(G38:AQ38,"M")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -19543,11 +19548,11 @@
         <v>9</v>
       </c>
       <c r="AR39">
-        <f>COUNTIF(G39:AQ39,"S")</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AS39">
-        <f>COUNTIF(G39:AQ39,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19616,11 +19621,11 @@
         <v>9</v>
       </c>
       <c r="AR40">
-        <f>COUNTIF(G40:AQ40,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS40">
-        <f>COUNTIF(G40:AQ40,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -19687,11 +19692,11 @@
       <c r="AP41" s="18"/>
       <c r="AQ41" s="18"/>
       <c r="AR41">
-        <f>COUNTIF(G41:AQ41,"S")</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AS41">
-        <f>COUNTIF(G41:AQ41,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -19762,11 +19767,11 @@
         <v>9</v>
       </c>
       <c r="AR42">
-        <f>COUNTIF(G42:AQ42,"S")</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AS42">
-        <f>COUNTIF(G42:AQ42,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -19841,11 +19846,11 @@
         <v>10</v>
       </c>
       <c r="AR43">
-        <f>COUNTIF(G43:AQ43,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS43">
-        <f>COUNTIF(G43:AQ43,"M")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -19924,11 +19929,11 @@
         <v>9</v>
       </c>
       <c r="AR44">
-        <f>COUNTIF(G44:AQ44,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS44">
-        <f>COUNTIF(G44:AQ44,"M")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
@@ -20003,11 +20008,11 @@
         <v>9</v>
       </c>
       <c r="AR45">
-        <f>COUNTIF(G45:AQ45,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS45">
-        <f>COUNTIF(G45:AQ45,"M")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -20084,11 +20089,11 @@
         <v>9</v>
       </c>
       <c r="AR46">
-        <f>COUNTIF(G46:AQ46,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS46">
-        <f>COUNTIF(G46:AQ46,"M")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -20165,11 +20170,11 @@
         <v>9</v>
       </c>
       <c r="AR47">
-        <f>COUNTIF(G47:AQ47,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS47">
-        <f>COUNTIF(G47:AQ47,"M")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -20242,11 +20247,11 @@
         <v>9</v>
       </c>
       <c r="AR48">
-        <f>COUNTIF(G48:AQ48,"S")</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AS48">
-        <f>COUNTIF(G48:AQ48,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -20313,11 +20318,11 @@
         <v>9</v>
       </c>
       <c r="AR49">
-        <f>COUNTIF(G49:AQ49,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS49">
-        <f>COUNTIF(G49:AQ49,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -20382,11 +20387,11 @@
       </c>
       <c r="AQ50" s="18"/>
       <c r="AR50">
-        <f>COUNTIF(G50:AQ50,"S")</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AS50">
-        <f>COUNTIF(G50:AQ50,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -20453,11 +20458,11 @@
       </c>
       <c r="AQ51" s="18"/>
       <c r="AR51">
-        <f>COUNTIF(G51:AQ51,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS51">
-        <f>COUNTIF(G51:AQ51,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -20528,11 +20533,11 @@
         <v>9</v>
       </c>
       <c r="AR52">
-        <f>COUNTIF(G52:AQ52,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS52">
-        <f>COUNTIF(G52:AQ52,"M")</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
@@ -20599,11 +20604,11 @@
         <v>9</v>
       </c>
       <c r="AR53">
-        <f>COUNTIF(G53:AQ53,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS53">
-        <f>COUNTIF(G53:AQ53,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -20672,11 +20677,11 @@
       <c r="AP54" s="18"/>
       <c r="AQ54" s="18"/>
       <c r="AR54">
-        <f>COUNTIF(G54:AQ54,"S")</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="AS54">
-        <f>COUNTIF(G54:AQ54,"M")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -20751,11 +20756,11 @@
         <v>9</v>
       </c>
       <c r="AR55">
-        <f>COUNTIF(G55:AQ55,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS55">
-        <f>COUNTIF(G55:AQ55,"M")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -20822,11 +20827,11 @@
         <v>9</v>
       </c>
       <c r="AR56">
-        <f>COUNTIF(G56:AQ56,"S")</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AS56">
-        <f>COUNTIF(G56:AQ56,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -20905,11 +20910,11 @@
         <v>10</v>
       </c>
       <c r="AR57">
-        <f>COUNTIF(G57:AQ57,"S")</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AS57">
-        <f>COUNTIF(G57:AQ57,"M")</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
@@ -20988,11 +20993,11 @@
       </c>
       <c r="AQ58" s="18"/>
       <c r="AR58">
-        <f>COUNTIF(G58:AQ58,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS58">
-        <f>COUNTIF(G58:AQ58,"M")</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
     </row>
@@ -21059,11 +21064,11 @@
       </c>
       <c r="AQ59" s="18"/>
       <c r="AR59">
-        <f>COUNTIF(G59:AQ59,"S")</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="AS59">
-        <f>COUNTIF(G59:AQ59,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -21148,11 +21153,11 @@
         <v>9</v>
       </c>
       <c r="AR60">
-        <f>COUNTIF(G60:AQ60,"S")</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AS60">
-        <f>COUNTIF(G60:AQ60,"M")</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -21227,11 +21232,11 @@
         <v>9</v>
       </c>
       <c r="AR61">
-        <f>COUNTIF(G61:AQ61,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS61">
-        <f>COUNTIF(G61:AQ61,"M")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -21302,11 +21307,11 @@
       <c r="AP62" s="18"/>
       <c r="AQ62" s="18"/>
       <c r="AR62">
-        <f>COUNTIF(G62:AQ62,"S")</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AS62">
-        <f>COUNTIF(G62:AQ62,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -21369,11 +21374,11 @@
       <c r="AP63" s="18"/>
       <c r="AQ63" s="18"/>
       <c r="AR63">
-        <f>COUNTIF(G63:AQ63,"S")</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AS63">
-        <f>COUNTIF(G63:AQ63,"M")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -21442,11 +21447,11 @@
         <v>9</v>
       </c>
       <c r="AR64">
-        <f>COUNTIF(G64:AQ64,"S")</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AS64">
-        <f>COUNTIF(G64:AQ64,"M")</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -21531,11 +21536,11 @@
         <v>9</v>
       </c>
       <c r="AR65">
-        <f>COUNTIF(G65:AQ65,"S")</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="AS65">
-        <f>COUNTIF(G65:AQ65,"M")</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
@@ -21602,11 +21607,11 @@
       <c r="AP66" s="18"/>
       <c r="AQ66" s="18"/>
       <c r="AR66">
-        <f>COUNTIF(G66:AQ66,"S")</f>
+        <f t="shared" ref="AR66:AR97" si="4">COUNTIF(G66:AQ66,"S")</f>
         <v>3</v>
       </c>
       <c r="AS66">
-        <f>COUNTIF(G66:AQ66,"M")</f>
+        <f t="shared" ref="AS66:AS101" si="5">COUNTIF(G66:AQ66,"M")</f>
         <v>0</v>
       </c>
     </row>
@@ -21689,11 +21694,11 @@
         <v>9</v>
       </c>
       <c r="AR67">
-        <f>COUNTIF(G67:AQ67,"S")</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="AS67">
-        <f>COUNTIF(G67:AQ67,"M")</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -21770,11 +21775,11 @@
       </c>
       <c r="AQ68" s="18"/>
       <c r="AR68">
-        <f>COUNTIF(G68:AQ68,"S")</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="AS68">
-        <f>COUNTIF(G68:AQ68,"M")</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -21845,11 +21850,11 @@
       </c>
       <c r="AQ69" s="18"/>
       <c r="AR69">
-        <f>COUNTIF(G69:AQ69,"S")</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AS69">
-        <f>COUNTIF(G69:AQ69,"M")</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -21912,11 +21917,11 @@
       <c r="AP70" s="18"/>
       <c r="AQ70" s="18"/>
       <c r="AR70">
-        <f>COUNTIF(G70:AQ70,"S")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AS70">
-        <f>COUNTIF(G70:AQ70,"M")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -21981,11 +21986,11 @@
       <c r="AP71" s="18"/>
       <c r="AQ71" s="18"/>
       <c r="AR71">
-        <f>COUNTIF(G71:AQ71,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS71">
-        <f>COUNTIF(G71:AQ71,"M")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22050,11 +22055,11 @@
       </c>
       <c r="AQ72" s="18"/>
       <c r="AR72">
-        <f>COUNTIF(G72:AQ72,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS72">
-        <f>COUNTIF(G72:AQ72,"M")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22123,11 +22128,11 @@
         <v>9</v>
       </c>
       <c r="AR73">
-        <f>COUNTIF(G73:AQ73,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS73">
-        <f>COUNTIF(G73:AQ73,"M")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -22196,11 +22201,11 @@
       <c r="AP74" s="18"/>
       <c r="AQ74" s="18"/>
       <c r="AR74">
-        <f>COUNTIF(G74:AQ74,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS74">
-        <f>COUNTIF(G74:AQ74,"M")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -22267,11 +22272,11 @@
       </c>
       <c r="AQ75" s="18"/>
       <c r="AR75">
-        <f>COUNTIF(G75:AQ75,"S")</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AS75">
-        <f>COUNTIF(G75:AQ75,"M")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22338,11 +22343,11 @@
       <c r="AP76" s="18"/>
       <c r="AQ76" s="18"/>
       <c r="AR76">
-        <f>COUNTIF(G76:AQ76,"S")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AS76">
-        <f>COUNTIF(G76:AQ76,"M")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -22421,11 +22426,11 @@
       </c>
       <c r="AQ77" s="18"/>
       <c r="AR77">
-        <f>COUNTIF(G77:AQ77,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS77">
-        <f>COUNTIF(G77:AQ77,"M")</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -22494,11 +22499,11 @@
       </c>
       <c r="AQ78" s="18"/>
       <c r="AR78">
-        <f>COUNTIF(G78:AQ78,"S")</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AS78">
-        <f>COUNTIF(G78:AQ78,"M")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -22571,11 +22576,11 @@
         <v>9</v>
       </c>
       <c r="AR79">
-        <f>COUNTIF(G79:AQ79,"S")</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AS79">
-        <f>COUNTIF(G79:AQ79,"M")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -22662,11 +22667,11 @@
       </c>
       <c r="AQ80" s="3"/>
       <c r="AR80">
-        <f>COUNTIF(G80:AQ80,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS80">
-        <f>COUNTIF(G80:AQ80,"M")</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
@@ -22739,11 +22744,11 @@
       <c r="AP81" s="18"/>
       <c r="AQ81" s="18"/>
       <c r="AR81">
-        <f>COUNTIF(G81:AQ81,"S")</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AS81">
-        <f>COUNTIF(G81:AQ81,"M")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -22828,11 +22833,11 @@
       </c>
       <c r="AQ82" s="3"/>
       <c r="AR82">
-        <f>COUNTIF(G82:AQ82,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS82">
-        <f>COUNTIF(G82:AQ82,"M")</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -22919,11 +22924,11 @@
       </c>
       <c r="AQ83" s="3"/>
       <c r="AR83">
-        <f>COUNTIF(G83:AQ83,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS83">
-        <f>COUNTIF(G83:AQ83,"M")</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
@@ -22996,11 +23001,11 @@
       </c>
       <c r="AQ84" s="18"/>
       <c r="AR84">
-        <f>COUNTIF(G84:AQ84,"S")</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="AS84">
-        <f>COUNTIF(G84:AQ84,"M")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -23067,11 +23072,11 @@
       <c r="AP85" s="18"/>
       <c r="AQ85" s="18"/>
       <c r="AR85">
-        <f>COUNTIF(G85:AQ85,"S")</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AS85">
-        <f>COUNTIF(G85:AQ85,"M")</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -23160,11 +23165,11 @@
       </c>
       <c r="AQ86" s="3"/>
       <c r="AR86">
-        <f>COUNTIF(G86:AQ86,"S")</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="AS86">
-        <f>COUNTIF(G86:AQ86,"M")</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -23253,11 +23258,11 @@
       </c>
       <c r="AQ87" s="3"/>
       <c r="AR87">
-        <f>COUNTIF(G87:AQ87,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS87">
-        <f>COUNTIF(G87:AQ87,"M")</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
@@ -23328,11 +23333,11 @@
       <c r="AP88" s="18"/>
       <c r="AQ88" s="18"/>
       <c r="AR88">
-        <f>COUNTIF(G88:AQ88,"S")</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AS88">
-        <f>COUNTIF(G88:AQ88,"M")</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -23427,11 +23432,11 @@
       </c>
       <c r="AQ89" s="18"/>
       <c r="AR89">
-        <f>COUNTIF(G89:AQ89,"S")</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="AS89">
-        <f>COUNTIF(G89:AQ89,"M")</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -23502,11 +23507,11 @@
       <c r="AP90" s="3"/>
       <c r="AQ90" s="3"/>
       <c r="AR90">
-        <f>COUNTIF(G90:AQ90,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS90">
-        <f>COUNTIF(G90:AQ90,"M")</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -23585,11 +23590,11 @@
       </c>
       <c r="AQ91" s="18"/>
       <c r="AR91">
-        <f>COUNTIF(G91:AQ91,"S")</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AS91">
-        <f>COUNTIF(G91:AQ91,"M")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -23686,11 +23691,11 @@
       </c>
       <c r="AQ92" s="3"/>
       <c r="AR92">
-        <f>COUNTIF(G92:AQ92,"S")</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="AS92">
-        <f>COUNTIF(G92:AQ92,"M")</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
@@ -23775,11 +23780,11 @@
       <c r="AP93" s="18"/>
       <c r="AQ93" s="18"/>
       <c r="AR93">
-        <f>COUNTIF(G93:AQ93,"S")</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AS93">
-        <f>COUNTIF(G93:AQ93,"M")</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
@@ -23854,11 +23859,11 @@
       <c r="AP94" s="3"/>
       <c r="AQ94" s="3"/>
       <c r="AR94">
-        <f>COUNTIF(G94:AQ94,"S")</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="AS94">
-        <f>COUNTIF(G94:AQ94,"M")</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -23947,11 +23952,11 @@
       <c r="AP95" s="3"/>
       <c r="AQ95" s="3"/>
       <c r="AR95">
-        <f>COUNTIF(G95:AQ95,"S")</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="AS95">
-        <f>COUNTIF(G95:AQ95,"M")</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -24036,11 +24041,11 @@
       <c r="AP96" s="18"/>
       <c r="AQ96" s="18"/>
       <c r="AR96">
-        <f>COUNTIF(G96:AQ96,"S")</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AS96">
-        <f>COUNTIF(G96:AQ96,"M")</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -24115,11 +24120,11 @@
       </c>
       <c r="AQ97" s="18"/>
       <c r="AR97">
-        <f>COUNTIF(G97:AQ97,"S")</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="AS97">
-        <f>COUNTIF(G97:AQ97,"M")</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -24210,11 +24215,11 @@
       </c>
       <c r="AQ98" s="18"/>
       <c r="AR98">
-        <f>COUNTIF(G98:AQ98,"S")</f>
+        <f t="shared" ref="AR98:AR129" si="6">COUNTIF(G98:AQ98,"S")</f>
         <v>7</v>
       </c>
       <c r="AS98">
-        <f>COUNTIF(G98:AQ98,"M")</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -24293,11 +24298,11 @@
       <c r="AP99" s="3"/>
       <c r="AQ99" s="3"/>
       <c r="AR99">
-        <f>COUNTIF(G99:AQ99,"S")</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="AS99">
-        <f>COUNTIF(G99:AQ99,"M")</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -24374,11 +24379,11 @@
       <c r="AP100" s="18"/>
       <c r="AQ100" s="18"/>
       <c r="AR100">
-        <f>COUNTIF(G100:AQ100,"S")</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="AS100">
-        <f>COUNTIF(G100:AQ100,"M")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>
@@ -24451,11 +24456,11 @@
       <c r="AP101" s="18"/>
       <c r="AQ101" s="18"/>
       <c r="AR101">
-        <f>COUNTIF(G101:AQ101,"S")</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AS101">
-        <f>COUNTIF(G101:AQ101,"M")</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
     </row>

</xml_diff>